<commit_message>
Poprawka w zadaniu 6
</commit_message>
<xml_diff>
--- a/matura2015/zadanie5.xlsx
+++ b/matura2015/zadanie5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="dane" sheetId="1" r:id="rId1"/>
@@ -471,11 +471,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="310009264"/>
-        <c:axId val="310010048"/>
+        <c:axId val="338721832"/>
+        <c:axId val="338722224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="310009264"/>
+        <c:axId val="338721832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +518,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310010048"/>
+        <c:crossAx val="338722224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -526,7 +526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310010048"/>
+        <c:axId val="338722224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +577,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310009264"/>
+        <c:crossAx val="338721832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1591,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,48 +1733,48 @@
         <v>1.0597000000000001</v>
       </c>
       <c r="M2">
-        <f>K2*L2</f>
-        <v>3158091.4475000002</v>
+        <f>ROUNDDOWN(K2*L2,0)</f>
+        <v>3158091</v>
       </c>
       <c r="N2">
-        <f>IF(M2&gt;$J2*2, M2, M2*$L2)</f>
-        <v>3346629.5069157504</v>
+        <f>IF(M2&gt;$J2*2, M2, ROUNDDOWN(M2*$L2, 0))</f>
+        <v>3346629</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:W2" si="0">IF(N2&gt;$J2*2, N2, N2*$L2)</f>
-        <v>3546423.2884786208</v>
+        <f t="shared" ref="O2:W2" si="0">IF(N2&gt;$J2*2, N2, ROUNDDOWN(N2*$L2, 0))</f>
+        <v>3546422</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>3758144.7588007948</v>
+        <v>3758143</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>3982506.0009012027</v>
+        <v>3982504</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>4220261.6091550048</v>
+        <v>4220259</v>
       </c>
       <c r="S2">
         <f t="shared" si="0"/>
-        <v>4472211.2272215588</v>
+        <v>4472208</v>
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>4739202.2374866866</v>
+        <v>4739198</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>5022132.6110646417</v>
+        <v>5022128</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>5321953.9279452013</v>
+        <v>5321949</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>5639674.5774435299</v>
+        <v>5639669</v>
       </c>
       <c r="X2">
         <f>K2*POWER(L2, 11)</f>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="Y2" t="b">
         <f>W2&lt;&gt;X2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1830,48 +1830,48 @@
         <v>0.93659999999999999</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M51" si="8">K3*L3</f>
-        <v>2941638.6258</v>
+        <f t="shared" ref="M3:M51" si="8">ROUNDDOWN(K3*L3,0)</f>
+        <v>2941638</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:W51" si="9">IF(M3&gt;$J3*2, M3, M3*$L3)</f>
-        <v>2755138.7369242799</v>
+        <f t="shared" ref="N3:W51" si="9">IF(M3&gt;$J3*2, M3, ROUNDDOWN(M3*$L3, 0))</f>
+        <v>2755138</v>
       </c>
       <c r="O3">
         <f t="shared" si="9"/>
-        <v>2580462.9410032807</v>
+        <v>2580462</v>
       </c>
       <c r="P3">
         <f t="shared" si="9"/>
-        <v>2416861.5905436724</v>
+        <v>2416860</v>
       </c>
       <c r="Q3">
         <f t="shared" si="9"/>
-        <v>2263632.5657032034</v>
+        <v>2263631</v>
       </c>
       <c r="R3">
         <f t="shared" si="9"/>
-        <v>2120118.2610376203</v>
+        <v>2120116</v>
       </c>
       <c r="S3">
         <f t="shared" si="9"/>
-        <v>1985702.7632878351</v>
+        <v>1985700</v>
       </c>
       <c r="T3">
         <f t="shared" si="9"/>
-        <v>1859809.2080953864</v>
+        <v>1859806</v>
       </c>
       <c r="U3">
         <f t="shared" si="9"/>
-        <v>1741897.304302139</v>
+        <v>1741894</v>
       </c>
       <c r="V3">
         <f t="shared" si="9"/>
-        <v>1631461.0152093833</v>
+        <v>1631457</v>
       </c>
       <c r="W3">
         <f t="shared" si="9"/>
-        <v>1528026.3868451084</v>
+        <v>1528022</v>
       </c>
       <c r="X3">
         <f t="shared" ref="X3:X51" si="10">K3*POWER(L3, 11)</f>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="Y3" t="b">
         <f t="shared" ref="Y3:Y51" si="11">W3&lt;&gt;X3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1928,47 +1928,47 @@
       </c>
       <c r="M4">
         <f t="shared" si="8"/>
-        <v>2540159.693</v>
+        <v>2540159</v>
       </c>
       <c r="N4">
         <f t="shared" si="9"/>
-        <v>2589692.8070135</v>
+        <v>2589692</v>
       </c>
       <c r="O4">
         <f t="shared" si="9"/>
-        <v>2640191.8167502633</v>
+        <v>2640190</v>
       </c>
       <c r="P4">
         <f t="shared" si="9"/>
-        <v>2691675.5571768936</v>
+        <v>2691673</v>
       </c>
       <c r="Q4">
         <f t="shared" si="9"/>
-        <v>2744163.230541843</v>
+        <v>2744160</v>
       </c>
       <c r="R4">
         <f t="shared" si="9"/>
-        <v>2797674.4135374092</v>
+        <v>2797671</v>
       </c>
       <c r="S4">
         <f t="shared" si="9"/>
-        <v>2852229.0646013888</v>
+        <v>2852225</v>
       </c>
       <c r="T4">
         <f t="shared" si="9"/>
-        <v>2907847.5313611161</v>
+        <v>2907843</v>
       </c>
       <c r="U4">
         <f t="shared" si="9"/>
-        <v>2964550.558222658</v>
+        <v>2964545</v>
       </c>
       <c r="V4">
         <f t="shared" si="9"/>
-        <v>3022359.2941080001</v>
+        <v>3022353</v>
       </c>
       <c r="W4">
         <f t="shared" si="9"/>
-        <v>3081295.3003431065</v>
+        <v>3081288</v>
       </c>
       <c r="X4">
         <f t="shared" si="10"/>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="Y4" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -2025,47 +2025,47 @@
       </c>
       <c r="M5">
         <f t="shared" si="8"/>
-        <v>1008345.27</v>
+        <v>1008345</v>
       </c>
       <c r="N5">
         <f t="shared" si="9"/>
-        <v>720462.69541500008</v>
+        <v>720462</v>
       </c>
       <c r="O5">
         <f t="shared" si="9"/>
-        <v>514770.59587401757</v>
+        <v>514770</v>
       </c>
       <c r="P5">
         <f t="shared" si="9"/>
-        <v>367803.59075198555</v>
+        <v>367803</v>
       </c>
       <c r="Q5">
         <f t="shared" si="9"/>
-        <v>262795.66559229366</v>
+        <v>262795</v>
       </c>
       <c r="R5">
         <f t="shared" si="9"/>
-        <v>187767.50306569383</v>
+        <v>187767</v>
       </c>
       <c r="S5">
         <f t="shared" si="9"/>
-        <v>134159.88094043825</v>
+        <v>134159</v>
       </c>
       <c r="T5">
         <f t="shared" si="9"/>
-        <v>95857.234931943138</v>
+        <v>95856</v>
       </c>
       <c r="U5">
         <f t="shared" si="9"/>
-        <v>68489.994358873373</v>
+        <v>68489</v>
       </c>
       <c r="V5">
         <f t="shared" si="9"/>
-        <v>48936.100969415027</v>
+        <v>48935</v>
       </c>
       <c r="W5">
         <f t="shared" si="9"/>
-        <v>34964.844142647038</v>
+        <v>34964</v>
       </c>
       <c r="X5">
         <f t="shared" si="10"/>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="Y5" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -2122,47 +2122,47 @@
       </c>
       <c r="M6">
         <f t="shared" si="8"/>
-        <v>3082698.8895999999</v>
+        <v>3082698</v>
       </c>
       <c r="N6">
         <f t="shared" si="9"/>
-        <v>2505925.9273558399</v>
+        <v>2505925</v>
       </c>
       <c r="O6">
         <f t="shared" si="9"/>
-        <v>2037067.1863475621</v>
+        <v>2037066</v>
       </c>
       <c r="P6">
         <f t="shared" si="9"/>
-        <v>1655931.9157819331</v>
+        <v>1655930</v>
       </c>
       <c r="Q6">
         <f t="shared" si="9"/>
-        <v>1346107.0543391334</v>
+        <v>1346105</v>
       </c>
       <c r="R6">
         <f t="shared" si="9"/>
-        <v>1094250.4244722815</v>
+        <v>1094248</v>
       </c>
       <c r="S6">
         <f t="shared" si="9"/>
-        <v>889516.17005351756</v>
+        <v>889514</v>
       </c>
       <c r="T6">
         <f t="shared" si="9"/>
-        <v>723087.6946365044</v>
+        <v>723085</v>
       </c>
       <c r="U6">
         <f t="shared" si="9"/>
-        <v>587797.9869700144</v>
+        <v>587795</v>
       </c>
       <c r="V6">
         <f t="shared" si="9"/>
-        <v>477820.98360792466</v>
+        <v>477818</v>
       </c>
       <c r="W6">
         <f t="shared" si="9"/>
-        <v>388420.67757488193</v>
+        <v>388418</v>
       </c>
       <c r="X6">
         <f t="shared" si="10"/>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="Y6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -2219,47 +2219,47 @@
       </c>
       <c r="M7">
         <f t="shared" si="8"/>
-        <v>4665074.3788000001</v>
+        <v>4665074</v>
       </c>
       <c r="N7">
         <f t="shared" si="9"/>
-        <v>5239345.0348302796</v>
+        <v>5239344</v>
       </c>
       <c r="O7">
         <f t="shared" si="9"/>
-        <v>5884308.4086178867</v>
+        <v>5884307</v>
       </c>
       <c r="P7">
         <f t="shared" si="9"/>
-        <v>6608666.7737187482</v>
+        <v>6608665</v>
       </c>
       <c r="Q7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="R7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="S7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="T7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="U7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="V7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="W7">
         <f t="shared" si="9"/>
-        <v>7422193.6535635265</v>
+        <v>7422191</v>
       </c>
       <c r="X7">
         <f t="shared" si="10"/>
@@ -2316,47 +2316,47 @@
       </c>
       <c r="M8">
         <f t="shared" si="8"/>
-        <v>5870402.5318</v>
+        <v>5870402</v>
       </c>
       <c r="N8">
         <f t="shared" si="9"/>
-        <v>5128970.6920336606</v>
+        <v>5128970</v>
       </c>
       <c r="O8">
         <f t="shared" si="9"/>
-        <v>4481181.6936298097</v>
+        <v>4481181</v>
       </c>
       <c r="P8">
         <f t="shared" si="9"/>
-        <v>3915208.4457243648</v>
+        <v>3915207</v>
       </c>
       <c r="Q8">
         <f t="shared" si="9"/>
-        <v>3420717.6190293776</v>
+        <v>3420716</v>
       </c>
       <c r="R8">
         <f t="shared" si="9"/>
-        <v>2988680.9837459675</v>
+        <v>2988679</v>
       </c>
       <c r="S8">
         <f t="shared" si="9"/>
-        <v>2611210.5754988519</v>
+        <v>2611208</v>
       </c>
       <c r="T8">
         <f t="shared" si="9"/>
-        <v>2281414.6798133468</v>
+        <v>2281412</v>
       </c>
       <c r="U8">
         <f t="shared" si="9"/>
-        <v>1993272.0057529211</v>
+        <v>1993269</v>
       </c>
       <c r="V8">
         <f t="shared" si="9"/>
-        <v>1741521.7514263273</v>
+        <v>1741519</v>
       </c>
       <c r="W8">
         <f t="shared" si="9"/>
-        <v>1521567.5542211821</v>
+        <v>1521565</v>
       </c>
       <c r="X8">
         <f t="shared" si="10"/>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="Y8" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -2413,47 +2413,47 @@
       </c>
       <c r="M9">
         <f t="shared" si="8"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="N9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="O9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="P9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="Q9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="R9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="S9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="T9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="U9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="V9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="W9">
         <f t="shared" si="9"/>
-        <v>3237471.7448</v>
+        <v>3237471</v>
       </c>
       <c r="X9">
         <f t="shared" si="10"/>
@@ -2510,47 +2510,47 @@
       </c>
       <c r="M10">
         <f t="shared" si="8"/>
-        <v>1484254.7254999999</v>
+        <v>1484254</v>
       </c>
       <c r="N10">
         <f t="shared" si="9"/>
-        <v>996677.04817324993</v>
+        <v>996676</v>
       </c>
       <c r="O10">
         <f t="shared" si="9"/>
-        <v>669268.6378483373</v>
+        <v>669267</v>
       </c>
       <c r="P10">
         <f t="shared" si="9"/>
-        <v>449413.89031515847</v>
+        <v>449412</v>
       </c>
       <c r="Q10">
         <f t="shared" si="9"/>
-        <v>301781.42734662892</v>
+        <v>301780</v>
       </c>
       <c r="R10">
         <f t="shared" si="9"/>
-        <v>202646.2284632613</v>
+        <v>202645</v>
       </c>
       <c r="S10">
         <f t="shared" si="9"/>
-        <v>136076.94241307996</v>
+        <v>136076</v>
       </c>
       <c r="T10">
         <f t="shared" si="9"/>
-        <v>91375.666830383198</v>
+        <v>91375</v>
       </c>
       <c r="U10">
         <f t="shared" si="9"/>
-        <v>61358.760276602319</v>
+        <v>61358</v>
       </c>
       <c r="V10">
         <f t="shared" si="9"/>
-        <v>41202.407525738454</v>
+        <v>41201</v>
       </c>
       <c r="W10">
         <f t="shared" si="9"/>
-        <v>27667.416653533372</v>
+        <v>27666</v>
       </c>
       <c r="X10">
         <f t="shared" si="10"/>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="Y10" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -2607,47 +2607,47 @@
       </c>
       <c r="M11">
         <f t="shared" si="8"/>
-        <v>1184004.3732</v>
+        <v>1184004</v>
       </c>
       <c r="N11">
         <f t="shared" si="9"/>
-        <v>842182.31065716012</v>
+        <v>842182</v>
       </c>
       <c r="O11">
         <f t="shared" si="9"/>
-        <v>599044.27757043799</v>
+        <v>599044</v>
       </c>
       <c r="P11">
         <f t="shared" si="9"/>
-        <v>426100.19463585259</v>
+        <v>426099</v>
       </c>
       <c r="Q11">
         <f t="shared" si="9"/>
-        <v>303085.06844448199</v>
+        <v>303084</v>
       </c>
       <c r="R11">
         <f t="shared" si="9"/>
-        <v>215584.40918456006</v>
+        <v>215583</v>
       </c>
       <c r="S11">
         <f t="shared" si="9"/>
-        <v>153345.19025297757</v>
+        <v>153344</v>
       </c>
       <c r="T11">
         <f t="shared" si="9"/>
-        <v>109074.43382694296</v>
+        <v>109073</v>
       </c>
       <c r="U11">
         <f t="shared" si="9"/>
-        <v>77584.644781104536</v>
+        <v>77583</v>
       </c>
       <c r="V11">
         <f t="shared" si="9"/>
-        <v>55185.957832799657</v>
+        <v>55184</v>
       </c>
       <c r="W11">
         <f t="shared" si="9"/>
-        <v>39253.771806470395</v>
+        <v>39252</v>
       </c>
       <c r="X11">
         <f t="shared" si="10"/>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="Y11" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -2704,47 +2704,47 @@
       </c>
       <c r="M12">
         <f t="shared" si="8"/>
-        <v>3532447.5962999999</v>
+        <v>3532447</v>
       </c>
       <c r="N12">
         <f t="shared" si="9"/>
-        <v>3326505.90143571</v>
+        <v>3326505</v>
       </c>
       <c r="O12">
         <f t="shared" si="9"/>
-        <v>3132570.6073820079</v>
+        <v>3132569</v>
       </c>
       <c r="P12">
         <f t="shared" si="9"/>
-        <v>2949941.740971637</v>
+        <v>2949940</v>
       </c>
       <c r="Q12">
         <f t="shared" si="9"/>
-        <v>2777960.1374729904</v>
+        <v>2777958</v>
       </c>
       <c r="R12">
         <f t="shared" si="9"/>
-        <v>2616005.0614583152</v>
+        <v>2616003</v>
       </c>
       <c r="S12">
         <f t="shared" si="9"/>
-        <v>2463491.9663752955</v>
+        <v>2463490</v>
       </c>
       <c r="T12">
         <f t="shared" si="9"/>
-        <v>2319870.3847356159</v>
+        <v>2319868</v>
       </c>
       <c r="U12">
         <f t="shared" si="9"/>
-        <v>2184621.9413055293</v>
+        <v>2184619</v>
       </c>
       <c r="V12">
         <f t="shared" si="9"/>
-        <v>2057258.4821274169</v>
+        <v>2057255</v>
       </c>
       <c r="W12">
         <f t="shared" si="9"/>
-        <v>1937320.3126193883</v>
+        <v>1937317</v>
       </c>
       <c r="X12">
         <f t="shared" si="10"/>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="Y12" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -2801,47 +2801,47 @@
       </c>
       <c r="M13">
         <f t="shared" si="8"/>
-        <v>10485718.240799999</v>
+        <v>10485718</v>
       </c>
       <c r="N13">
         <f t="shared" si="9"/>
-        <v>12245221.761606239</v>
+        <v>12245221</v>
       </c>
       <c r="O13">
         <f t="shared" si="9"/>
-        <v>14299969.973203765</v>
+        <v>14299969</v>
       </c>
       <c r="P13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="Q13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="R13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="S13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="T13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="U13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="V13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="W13">
         <f t="shared" si="9"/>
-        <v>16699504.934707357</v>
+        <v>16699503</v>
       </c>
       <c r="X13">
         <f t="shared" si="10"/>
@@ -2898,47 +2898,47 @@
       </c>
       <c r="M14">
         <f t="shared" si="8"/>
-        <v>2339080.7121000001</v>
+        <v>2339080</v>
       </c>
       <c r="N14">
         <f t="shared" si="9"/>
-        <v>2554977.8618268301</v>
+        <v>2554977</v>
       </c>
       <c r="O14">
         <f t="shared" si="9"/>
-        <v>2790802.3184734466</v>
+        <v>2790801</v>
       </c>
       <c r="P14">
         <f t="shared" si="9"/>
-        <v>3048393.372468546</v>
+        <v>3048391</v>
       </c>
       <c r="Q14">
         <f t="shared" si="9"/>
-        <v>3329760.080747393</v>
+        <v>3329757</v>
       </c>
       <c r="R14">
         <f t="shared" si="9"/>
-        <v>3637096.9362003775</v>
+        <v>3637093</v>
       </c>
       <c r="S14">
         <f t="shared" si="9"/>
-        <v>3972800.9834116725</v>
+        <v>3972796</v>
       </c>
       <c r="T14">
         <f t="shared" si="9"/>
-        <v>3972800.9834116725</v>
+        <v>3972796</v>
       </c>
       <c r="U14">
         <f t="shared" si="9"/>
-        <v>3972800.9834116725</v>
+        <v>3972796</v>
       </c>
       <c r="V14">
         <f t="shared" si="9"/>
-        <v>3972800.9834116725</v>
+        <v>3972796</v>
       </c>
       <c r="W14">
         <f t="shared" si="9"/>
-        <v>3972800.9834116725</v>
+        <v>3972796</v>
       </c>
       <c r="X14">
         <f t="shared" si="10"/>
@@ -2995,47 +2995,47 @@
       </c>
       <c r="M15">
         <f t="shared" si="8"/>
-        <v>1431954.5247</v>
+        <v>1431954</v>
       </c>
       <c r="N15">
         <f t="shared" si="9"/>
-        <v>1161171.9240792298</v>
+        <v>1161171</v>
       </c>
       <c r="O15">
         <f t="shared" si="9"/>
-        <v>941594.3132358474</v>
+        <v>941593</v>
       </c>
       <c r="P15">
         <f t="shared" si="9"/>
-        <v>763538.82860294858</v>
+        <v>763537</v>
       </c>
       <c r="Q15">
         <f t="shared" si="9"/>
-        <v>619153.63611413096</v>
+        <v>619152</v>
       </c>
       <c r="R15">
         <f t="shared" si="9"/>
-        <v>502071.68352494878</v>
+        <v>502070</v>
       </c>
       <c r="S15">
         <f t="shared" si="9"/>
-        <v>407129.92817038094</v>
+        <v>407128</v>
       </c>
       <c r="T15">
         <f t="shared" si="9"/>
-        <v>330141.6587533619</v>
+        <v>330140</v>
       </c>
       <c r="U15">
         <f t="shared" si="9"/>
-        <v>267711.87108310114</v>
+        <v>267710</v>
       </c>
       <c r="V15">
         <f t="shared" si="9"/>
-        <v>217087.55626128669</v>
+        <v>217086</v>
       </c>
       <c r="W15">
         <f t="shared" si="9"/>
-        <v>176036.29937227737</v>
+        <v>176035</v>
       </c>
       <c r="X15">
         <f t="shared" si="10"/>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="Y15" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -3092,47 +3092,47 @@
       </c>
       <c r="M16">
         <f t="shared" si="8"/>
-        <v>3273847.6044999999</v>
+        <v>3273847</v>
       </c>
       <c r="N16">
         <f t="shared" si="9"/>
-        <v>2614167.3121932498</v>
+        <v>2614166</v>
       </c>
       <c r="O16">
         <f t="shared" si="9"/>
-        <v>2087412.5987863101</v>
+        <v>2087411</v>
       </c>
       <c r="P16">
         <f t="shared" si="9"/>
-        <v>1666798.9601308685</v>
+        <v>1666797</v>
       </c>
       <c r="Q16">
         <f t="shared" si="9"/>
-        <v>1330938.9696644985</v>
+        <v>1330937</v>
       </c>
       <c r="R16">
         <f t="shared" si="9"/>
-        <v>1062754.767277102</v>
+        <v>1062753</v>
       </c>
       <c r="S16">
         <f t="shared" si="9"/>
-        <v>848609.68167076597</v>
+        <v>848608</v>
       </c>
       <c r="T16">
         <f t="shared" si="9"/>
-        <v>677614.83081410662</v>
+        <v>677613</v>
       </c>
       <c r="U16">
         <f t="shared" si="9"/>
-        <v>541075.44240506412</v>
+        <v>541073</v>
       </c>
       <c r="V16">
         <f t="shared" si="9"/>
-        <v>432048.74076044367</v>
+        <v>432046</v>
       </c>
       <c r="W16">
         <f t="shared" si="9"/>
-        <v>344990.91949721426</v>
+        <v>344988</v>
       </c>
       <c r="X16">
         <f t="shared" si="10"/>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="Y16" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -3189,47 +3189,47 @@
       </c>
       <c r="M17">
         <f t="shared" si="8"/>
-        <v>4257995.6376</v>
+        <v>4257995</v>
       </c>
       <c r="N17">
         <f t="shared" si="9"/>
-        <v>5319088.1504899208</v>
+        <v>5319087</v>
       </c>
       <c r="O17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="P17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="Q17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="R17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="S17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="T17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="U17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="V17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="W17">
         <f t="shared" si="9"/>
-        <v>6644604.9175920095</v>
+        <v>6644603</v>
       </c>
       <c r="X17">
         <f t="shared" si="10"/>
@@ -3286,47 +3286,47 @@
       </c>
       <c r="M18">
         <f t="shared" si="8"/>
-        <v>1821628.0259999998</v>
+        <v>1821628</v>
       </c>
       <c r="N18">
         <f t="shared" si="9"/>
-        <v>1098441.6996779998</v>
+        <v>1098441</v>
       </c>
       <c r="O18">
         <f t="shared" si="9"/>
-        <v>662360.34490583383</v>
+        <v>662359</v>
       </c>
       <c r="P18">
         <f t="shared" si="9"/>
-        <v>399403.28797821776</v>
+        <v>399402</v>
       </c>
       <c r="Q18">
         <f t="shared" si="9"/>
-        <v>240840.18265086529</v>
+        <v>240839</v>
       </c>
       <c r="R18">
         <f t="shared" si="9"/>
-        <v>145226.63013847175</v>
+        <v>145225</v>
       </c>
       <c r="S18">
         <f t="shared" si="9"/>
-        <v>87571.65797349847</v>
+        <v>87570</v>
       </c>
       <c r="T18">
         <f t="shared" si="9"/>
-        <v>52805.709758019577</v>
+        <v>52804</v>
       </c>
       <c r="U18">
         <f t="shared" si="9"/>
-        <v>31841.842984085804</v>
+        <v>31840</v>
       </c>
       <c r="V18">
         <f t="shared" si="9"/>
-        <v>19200.631319403739</v>
+        <v>19199</v>
       </c>
       <c r="W18">
         <f t="shared" si="9"/>
-        <v>11577.980685600454</v>
+        <v>11576</v>
       </c>
       <c r="X18">
         <f t="shared" si="10"/>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="Y18" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -3383,47 +3383,47 @@
       </c>
       <c r="M19">
         <f t="shared" si="8"/>
-        <v>578283.17539999995</v>
+        <v>578283</v>
       </c>
       <c r="N19">
         <f t="shared" si="9"/>
-        <v>266183.74563661998</v>
+        <v>266183</v>
       </c>
       <c r="O19">
         <f t="shared" si="9"/>
-        <v>122524.37811653617</v>
+        <v>122524</v>
       </c>
       <c r="P19">
         <f t="shared" si="9"/>
-        <v>56397.971247041598</v>
+        <v>56397</v>
       </c>
       <c r="Q19">
         <f t="shared" si="9"/>
-        <v>25959.986165013248</v>
+        <v>25959</v>
       </c>
       <c r="R19">
         <f t="shared" si="9"/>
-        <v>11949.381631755597</v>
+        <v>11948</v>
       </c>
       <c r="S19">
         <f t="shared" si="9"/>
-        <v>5500.3003650971013</v>
+        <v>5499</v>
       </c>
       <c r="T19">
         <f t="shared" si="9"/>
-        <v>2531.7882580541955</v>
+        <v>2531</v>
       </c>
       <c r="U19">
         <f t="shared" si="9"/>
-        <v>1165.3821351823462</v>
+        <v>1165</v>
       </c>
       <c r="V19">
         <f t="shared" si="9"/>
-        <v>536.42539682443396</v>
+        <v>536</v>
       </c>
       <c r="W19">
         <f t="shared" si="9"/>
-        <v>246.91661015828694</v>
+        <v>246</v>
       </c>
       <c r="X19">
         <f t="shared" si="10"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="Y19" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -3480,47 +3480,47 @@
       </c>
       <c r="M20">
         <f t="shared" si="8"/>
-        <v>1899902.6481999999</v>
+        <v>1899902</v>
       </c>
       <c r="N20">
         <f t="shared" si="9"/>
-        <v>1053686.00869172</v>
+        <v>1053685</v>
       </c>
       <c r="O20">
         <f t="shared" si="9"/>
-        <v>584374.26042042789</v>
+        <v>584373</v>
       </c>
       <c r="P20">
         <f t="shared" si="9"/>
-        <v>324093.96482916927</v>
+        <v>324093</v>
       </c>
       <c r="Q20">
         <f t="shared" si="9"/>
-        <v>179742.51289425726</v>
+        <v>179741</v>
       </c>
       <c r="R20">
         <f t="shared" si="9"/>
-        <v>99685.197651155075</v>
+        <v>99684</v>
       </c>
       <c r="S20">
         <f t="shared" si="9"/>
-        <v>55285.410617330599</v>
+        <v>55284</v>
       </c>
       <c r="T20">
         <f t="shared" si="9"/>
-        <v>30661.28872837155</v>
+        <v>30660</v>
       </c>
       <c r="U20">
         <f t="shared" si="9"/>
-        <v>17004.750728754861</v>
+        <v>17004</v>
       </c>
       <c r="V20">
         <f t="shared" si="9"/>
-        <v>9430.8347541674466</v>
+        <v>9430</v>
       </c>
       <c r="W20">
         <f t="shared" si="9"/>
-        <v>5230.3409546612656</v>
+        <v>5229</v>
       </c>
       <c r="X20">
         <f t="shared" si="10"/>
@@ -3577,47 +3577,47 @@
       </c>
       <c r="M21">
         <f t="shared" si="8"/>
-        <v>2565842.3459999999</v>
+        <v>2565842</v>
       </c>
       <c r="N21">
         <f t="shared" si="9"/>
-        <v>2369298.8222964001</v>
+        <v>2369298</v>
       </c>
       <c r="O21">
         <f t="shared" si="9"/>
-        <v>2187810.5325084957</v>
+        <v>2187809</v>
       </c>
       <c r="P21">
         <f t="shared" si="9"/>
-        <v>2020224.245718345</v>
+        <v>2020222</v>
       </c>
       <c r="Q21">
         <f t="shared" si="9"/>
-        <v>1865475.0684963197</v>
+        <v>1865472</v>
       </c>
       <c r="R21">
         <f t="shared" si="9"/>
-        <v>1722579.6782495016</v>
+        <v>1722576</v>
       </c>
       <c r="S21">
         <f t="shared" si="9"/>
-        <v>1590630.0748955898</v>
+        <v>1590626</v>
       </c>
       <c r="T21">
         <f t="shared" si="9"/>
-        <v>1468787.8111585877</v>
+        <v>1468784</v>
       </c>
       <c r="U21">
         <f t="shared" si="9"/>
-        <v>1356278.6648238399</v>
+        <v>1356275</v>
       </c>
       <c r="V21">
         <f t="shared" si="9"/>
-        <v>1252387.7190983337</v>
+        <v>1252384</v>
       </c>
       <c r="W21">
         <f t="shared" si="9"/>
-        <v>1156454.8198154015</v>
+        <v>1156451</v>
       </c>
       <c r="X21">
         <f t="shared" si="10"/>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="Y21" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -3661,11 +3661,11 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f t="shared" si="5"/>
+        <f>B22 + C22</f>
         <v>4752576</v>
       </c>
       <c r="K22">
-        <f t="shared" si="6"/>
+        <f>D22+E22</f>
         <v>572183</v>
       </c>
       <c r="L22">
@@ -3674,47 +3674,47 @@
       </c>
       <c r="M22">
         <f t="shared" si="8"/>
-        <v>68833.6149</v>
+        <v>68833</v>
       </c>
       <c r="N22">
         <f t="shared" si="9"/>
-        <v>8280.683872470001</v>
+        <v>8280</v>
       </c>
       <c r="O22">
         <f t="shared" si="9"/>
-        <v>996.16626985814116</v>
+        <v>996</v>
       </c>
       <c r="P22">
         <f t="shared" si="9"/>
-        <v>119.83880226393438</v>
+        <v>119</v>
       </c>
       <c r="Q22">
         <f t="shared" si="9"/>
-        <v>14.416607912351306</v>
+        <v>14</v>
       </c>
       <c r="R22">
         <f t="shared" si="9"/>
-        <v>1.7343179318558621</v>
+        <v>1</v>
       </c>
       <c r="S22">
         <f t="shared" si="9"/>
-        <v>0.20863844720226021</v>
+        <v>0</v>
       </c>
       <c r="T22">
         <f t="shared" si="9"/>
-        <v>2.5099205198431906E-2</v>
+        <v>0</v>
       </c>
       <c r="U22">
         <f t="shared" si="9"/>
-        <v>3.0194343853713582E-3</v>
+        <v>0</v>
       </c>
       <c r="V22">
         <f t="shared" si="9"/>
-        <v>3.6323795656017442E-4</v>
+        <v>0</v>
       </c>
       <c r="W22">
         <f t="shared" si="9"/>
-        <v>4.3697526174188982E-5</v>
+        <v>0</v>
       </c>
       <c r="X22">
         <f t="shared" si="10"/>
@@ -3722,7 +3722,7 @@
       </c>
       <c r="Y22" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -3771,47 +3771,47 @@
       </c>
       <c r="M23">
         <f t="shared" si="8"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="N23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="O23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="P23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="Q23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="R23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="S23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="T23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="U23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="V23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="W23">
         <f t="shared" si="9"/>
-        <v>21234122.037100002</v>
+        <v>21234122</v>
       </c>
       <c r="X23">
         <f t="shared" si="10"/>
@@ -3868,47 +3868,47 @@
       </c>
       <c r="M24">
         <f t="shared" si="8"/>
-        <v>2378798.3015999999</v>
+        <v>2378798</v>
       </c>
       <c r="N24">
         <f t="shared" si="9"/>
-        <v>1728434.8459425599</v>
+        <v>1728434</v>
       </c>
       <c r="O24">
         <f t="shared" si="9"/>
-        <v>1255880.7590618641</v>
+        <v>1255880</v>
       </c>
       <c r="P24">
         <f t="shared" si="9"/>
-        <v>912522.95953435055</v>
+        <v>912522</v>
       </c>
       <c r="Q24">
         <f t="shared" si="9"/>
-        <v>663039.18239765917</v>
+        <v>663038</v>
       </c>
       <c r="R24">
         <f t="shared" si="9"/>
-        <v>481764.26993013918</v>
+        <v>481763</v>
       </c>
       <c r="S24">
         <f t="shared" si="9"/>
-        <v>350049.91853123915</v>
+        <v>350048</v>
       </c>
       <c r="T24">
         <f t="shared" si="9"/>
-        <v>254346.27080479838</v>
+        <v>254344</v>
       </c>
       <c r="U24">
         <f t="shared" si="9"/>
-        <v>184808.0003667665</v>
+        <v>184806</v>
       </c>
       <c r="V24">
         <f t="shared" si="9"/>
-        <v>134281.49306649255</v>
+        <v>134280</v>
       </c>
       <c r="W24">
         <f t="shared" si="9"/>
-        <v>97568.932862113492</v>
+        <v>97567</v>
       </c>
       <c r="X24">
         <f t="shared" si="10"/>
@@ -3965,47 +3965,47 @@
       </c>
       <c r="M25">
         <f t="shared" si="8"/>
-        <v>2086303.4829000002</v>
+        <v>2086303</v>
       </c>
       <c r="N25">
         <f t="shared" si="9"/>
-        <v>2615598.6765117301</v>
+        <v>2615598</v>
       </c>
       <c r="O25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="P25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="Q25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="R25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="S25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="T25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="U25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="V25">
         <f t="shared" si="9"/>
-        <v>3279176.0607427559</v>
+        <v>3279175</v>
       </c>
       <c r="W25">
-        <f t="shared" ref="O25:W40" si="12">IF(V25&gt;$J25*2, V25, V25*$L25)</f>
-        <v>3279176.0607427559</v>
+        <f t="shared" ref="O25:W40" si="12">IF(V25&gt;$J25*2, V25, ROUNDDOWN(V25*$L25, 0))</f>
+        <v>3279175</v>
       </c>
       <c r="X25">
         <f t="shared" si="10"/>
@@ -4062,47 +4062,47 @@
       </c>
       <c r="M26">
         <f t="shared" si="8"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="N26">
         <f t="shared" si="9"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="O26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="P26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="Q26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="R26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="S26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="T26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="U26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="V26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="W26">
         <f t="shared" si="12"/>
-        <v>12662049.239599999</v>
+        <v>12662049</v>
       </c>
       <c r="X26">
         <f t="shared" si="10"/>
@@ -4159,47 +4159,47 @@
       </c>
       <c r="M27">
         <f t="shared" si="8"/>
-        <v>1622245.7582999999</v>
+        <v>1622245</v>
       </c>
       <c r="N27">
         <f t="shared" si="9"/>
-        <v>1408595.9919318899</v>
+        <v>1408595</v>
       </c>
       <c r="O27">
         <f t="shared" si="12"/>
-        <v>1223083.89979446</v>
+        <v>1223083</v>
       </c>
       <c r="P27">
         <f t="shared" si="12"/>
-        <v>1062003.7501915295</v>
+        <v>1062002</v>
       </c>
       <c r="Q27">
         <f t="shared" si="12"/>
-        <v>922137.85629130504</v>
+        <v>922136</v>
       </c>
       <c r="R27">
         <f t="shared" si="12"/>
-        <v>800692.30061774014</v>
+        <v>800690</v>
       </c>
       <c r="S27">
         <f t="shared" si="12"/>
-        <v>695241.12462638377</v>
+        <v>695239</v>
       </c>
       <c r="T27">
         <f t="shared" si="12"/>
-        <v>603677.86851308902</v>
+        <v>603676</v>
       </c>
       <c r="U27">
         <f t="shared" si="12"/>
-        <v>524173.49322991516</v>
+        <v>524171</v>
       </c>
       <c r="V27">
         <f t="shared" si="12"/>
-        <v>455139.84417153528</v>
+        <v>455137</v>
       </c>
       <c r="W27">
         <f t="shared" si="12"/>
-        <v>395197.92669414409</v>
+        <v>395195</v>
       </c>
       <c r="X27">
         <f t="shared" si="10"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="Y27" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -4256,47 +4256,47 @@
       </c>
       <c r="M28">
         <f t="shared" si="8"/>
-        <v>1046225.6736</v>
+        <v>1046225</v>
       </c>
       <c r="N28">
         <f t="shared" si="9"/>
-        <v>493086.15996768</v>
+        <v>493085</v>
       </c>
       <c r="O28">
         <f t="shared" si="12"/>
-        <v>232391.50719276757</v>
+        <v>232390</v>
       </c>
       <c r="P28">
         <f t="shared" si="12"/>
-        <v>109526.11733995135</v>
+        <v>109525</v>
       </c>
       <c r="Q28">
         <f t="shared" si="12"/>
-        <v>51619.65910231907</v>
+        <v>51619</v>
       </c>
       <c r="R28">
         <f t="shared" si="12"/>
-        <v>24328.345334922979</v>
+        <v>24328</v>
       </c>
       <c r="S28">
         <f t="shared" si="12"/>
-        <v>11465.949156349199</v>
+        <v>11465</v>
       </c>
       <c r="T28">
         <f t="shared" si="12"/>
-        <v>5403.9018373873778</v>
+        <v>5403</v>
       </c>
       <c r="U28">
         <f t="shared" si="12"/>
-        <v>2546.8589359606713</v>
+        <v>2546</v>
       </c>
       <c r="V28">
         <f t="shared" si="12"/>
-        <v>1200.3346165182643</v>
+        <v>1199</v>
       </c>
       <c r="W28">
         <f t="shared" si="12"/>
-        <v>565.71770476505799</v>
+        <v>565</v>
       </c>
       <c r="X28">
         <f t="shared" si="10"/>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="Y28" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -4353,47 +4353,47 @@
       </c>
       <c r="M29">
         <f t="shared" si="8"/>
-        <v>137316.28590000002</v>
+        <v>137316</v>
       </c>
       <c r="N29">
         <f t="shared" si="9"/>
-        <v>21792.094572330003</v>
+        <v>21792</v>
       </c>
       <c r="O29">
         <f t="shared" si="12"/>
-        <v>3458.4054086287715</v>
+        <v>3458</v>
       </c>
       <c r="P29">
         <f t="shared" si="12"/>
-        <v>548.84893834938612</v>
+        <v>548</v>
       </c>
       <c r="Q29">
         <f t="shared" si="12"/>
-        <v>87.102326516047583</v>
+        <v>86</v>
       </c>
       <c r="R29">
         <f t="shared" si="12"/>
-        <v>13.823139218096753</v>
+        <v>13</v>
       </c>
       <c r="S29">
         <f t="shared" si="12"/>
-        <v>2.1937321939119547</v>
+        <v>2</v>
       </c>
       <c r="T29">
         <f t="shared" si="12"/>
-        <v>0.34814529917382725</v>
+        <v>0</v>
       </c>
       <c r="U29">
         <f t="shared" si="12"/>
-        <v>5.525065897888639E-2</v>
+        <v>0</v>
       </c>
       <c r="V29">
         <f t="shared" si="12"/>
-        <v>8.7682795799492712E-3</v>
+        <v>0</v>
       </c>
       <c r="W29">
         <f t="shared" si="12"/>
-        <v>1.3915259693379493E-3</v>
+        <v>0</v>
       </c>
       <c r="X29">
         <f t="shared" si="10"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="Y29" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -4450,47 +4450,47 @@
       </c>
       <c r="M30">
         <f t="shared" si="8"/>
-        <v>2503921.3023999999</v>
+        <v>2503921</v>
       </c>
       <c r="N30">
         <f t="shared" si="9"/>
-        <v>2058724.09483328</v>
+        <v>2058723</v>
       </c>
       <c r="O30">
         <f t="shared" si="12"/>
-        <v>1692682.9507719229</v>
+        <v>1692682</v>
       </c>
       <c r="P30">
         <f t="shared" si="12"/>
-        <v>1391723.922124675</v>
+        <v>1391723</v>
       </c>
       <c r="Q30">
         <f t="shared" si="12"/>
-        <v>1144275.4087709079</v>
+        <v>1144274</v>
       </c>
       <c r="R30">
         <f t="shared" si="12"/>
-        <v>940823.24109144055</v>
+        <v>940822</v>
       </c>
       <c r="S30">
         <f t="shared" si="12"/>
-        <v>773544.86882538244</v>
+        <v>773543</v>
       </c>
       <c r="T30">
         <f t="shared" si="12"/>
-        <v>636008.59114822943</v>
+        <v>636007</v>
       </c>
       <c r="U30">
         <f t="shared" si="12"/>
-        <v>522926.26364207425</v>
+        <v>522924</v>
       </c>
       <c r="V30">
         <f t="shared" si="12"/>
-        <v>429949.97396651347</v>
+        <v>429948</v>
       </c>
       <c r="W30">
         <f t="shared" si="12"/>
-        <v>353504.86859526741</v>
+        <v>353503</v>
       </c>
       <c r="X30">
         <f t="shared" si="10"/>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="Y30" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -4547,47 +4547,47 @@
       </c>
       <c r="M31">
         <f t="shared" si="8"/>
-        <v>695.34270000000004</v>
+        <v>695</v>
       </c>
       <c r="N31">
         <f t="shared" si="9"/>
-        <v>8.1355095899999998</v>
+        <v>8</v>
       </c>
       <c r="O31">
         <f t="shared" si="12"/>
-        <v>9.5185462203000004E-2</v>
+        <v>0</v>
       </c>
       <c r="P31">
         <f t="shared" si="12"/>
-        <v>1.1136699077751002E-3</v>
+        <v>0</v>
       </c>
       <c r="Q31">
         <f t="shared" si="12"/>
-        <v>1.3029937920968673E-5</v>
+        <v>0</v>
       </c>
       <c r="R31">
         <f t="shared" si="12"/>
-        <v>1.5245027367533347E-7</v>
+        <v>0</v>
       </c>
       <c r="S31">
         <f t="shared" si="12"/>
-        <v>1.7836682020014017E-9</v>
+        <v>0</v>
       </c>
       <c r="T31">
         <f t="shared" si="12"/>
-        <v>2.08689179634164E-11</v>
+        <v>0</v>
       </c>
       <c r="U31">
         <f t="shared" si="12"/>
-        <v>2.4416634017197187E-13</v>
+        <v>0</v>
       </c>
       <c r="V31">
         <f t="shared" si="12"/>
-        <v>2.8567461800120708E-15</v>
+        <v>0</v>
       </c>
       <c r="W31">
         <f t="shared" si="12"/>
-        <v>3.342393030614123E-17</v>
+        <v>0</v>
       </c>
       <c r="X31">
         <f t="shared" si="10"/>
@@ -4595,7 +4595,7 @@
       </c>
       <c r="Y31" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -4644,47 +4644,47 @@
       </c>
       <c r="M32">
         <f t="shared" si="8"/>
-        <v>3220584.0597000001</v>
+        <v>3220584</v>
       </c>
       <c r="N32">
         <f t="shared" si="9"/>
-        <v>2982582.8976881704</v>
+        <v>2982582</v>
       </c>
       <c r="O32">
         <f t="shared" si="12"/>
-        <v>2762170.0215490148</v>
+        <v>2762169</v>
       </c>
       <c r="P32">
         <f t="shared" si="12"/>
-        <v>2558045.6569565427</v>
+        <v>2558044</v>
       </c>
       <c r="Q32">
         <f t="shared" si="12"/>
-        <v>2369006.0829074541</v>
+        <v>2369004</v>
       </c>
       <c r="R32">
         <f t="shared" si="12"/>
-        <v>2193936.5333805932</v>
+        <v>2193934</v>
       </c>
       <c r="S32">
         <f t="shared" si="12"/>
-        <v>2031804.6235637674</v>
+        <v>2031802</v>
       </c>
       <c r="T32">
         <f t="shared" si="12"/>
-        <v>1881654.261882405</v>
+        <v>1881651</v>
       </c>
       <c r="U32">
         <f t="shared" si="12"/>
-        <v>1742600.0119292953</v>
+        <v>1742596</v>
       </c>
       <c r="V32">
         <f t="shared" si="12"/>
-        <v>1613821.8710477203</v>
+        <v>1613818</v>
       </c>
       <c r="W32">
         <f t="shared" si="12"/>
-        <v>1494560.4347772938</v>
+        <v>1494556</v>
       </c>
       <c r="X32">
         <f t="shared" si="10"/>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="Y32" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -4741,47 +4741,47 @@
       </c>
       <c r="M33">
         <f t="shared" si="8"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="N33">
         <f t="shared" si="9"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="O33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="P33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="Q33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="R33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="S33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="T33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="U33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="V33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="W33">
         <f t="shared" si="12"/>
-        <v>7356805.1629999997</v>
+        <v>7356805</v>
       </c>
       <c r="X33">
         <f t="shared" si="10"/>
@@ -4838,47 +4838,47 @@
       </c>
       <c r="M34">
         <f t="shared" si="8"/>
-        <v>153706.734</v>
+        <v>153706</v>
       </c>
       <c r="N34">
         <f t="shared" si="9"/>
-        <v>24900.490908</v>
+        <v>24900</v>
       </c>
       <c r="O34">
         <f t="shared" si="12"/>
-        <v>4033.8795270959999</v>
+        <v>4033</v>
       </c>
       <c r="P34">
         <f t="shared" si="12"/>
-        <v>653.48848338955202</v>
+        <v>653</v>
       </c>
       <c r="Q34">
         <f t="shared" si="12"/>
-        <v>105.86513430910743</v>
+        <v>105</v>
       </c>
       <c r="R34">
         <f t="shared" si="12"/>
-        <v>17.150151758075406</v>
+        <v>17</v>
       </c>
       <c r="S34">
         <f t="shared" si="12"/>
-        <v>2.7783245848082161</v>
+        <v>2</v>
       </c>
       <c r="T34">
         <f t="shared" si="12"/>
-        <v>0.45008858273893104</v>
+        <v>0</v>
       </c>
       <c r="U34">
         <f t="shared" si="12"/>
-        <v>7.2914350403706835E-2</v>
+        <v>0</v>
       </c>
       <c r="V34">
         <f t="shared" si="12"/>
-        <v>1.1812124765400507E-2</v>
+        <v>0</v>
       </c>
       <c r="W34">
         <f t="shared" si="12"/>
-        <v>1.9135642119948821E-3</v>
+        <v>0</v>
       </c>
       <c r="X34">
         <f t="shared" si="10"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="Y34" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -4935,47 +4935,47 @@
       </c>
       <c r="M35">
         <f t="shared" si="8"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="N35">
         <f t="shared" si="9"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="O35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="P35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="Q35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="R35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="S35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="T35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="U35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="V35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="W35">
         <f t="shared" si="12"/>
-        <v>48002606.409999996</v>
+        <v>48002606</v>
       </c>
       <c r="X35">
         <f t="shared" si="10"/>
@@ -5032,47 +5032,47 @@
       </c>
       <c r="M36">
         <f t="shared" si="8"/>
-        <v>791631.80650000006</v>
+        <v>791631</v>
       </c>
       <c r="N36">
         <f t="shared" si="9"/>
-        <v>315465.27489025006</v>
+        <v>315464</v>
       </c>
       <c r="O36">
         <f t="shared" si="12"/>
-        <v>125712.91204376465</v>
+        <v>125712</v>
       </c>
       <c r="P36">
         <f t="shared" si="12"/>
-        <v>50096.595449440218</v>
+        <v>50096</v>
       </c>
       <c r="Q36">
         <f t="shared" si="12"/>
-        <v>19963.493286601926</v>
+        <v>19963</v>
       </c>
       <c r="R36">
         <f t="shared" si="12"/>
-        <v>7955.4520747108681</v>
+        <v>7955</v>
       </c>
       <c r="S36">
         <f t="shared" si="12"/>
-        <v>3170.2476517722812</v>
+        <v>3170</v>
       </c>
       <c r="T36">
         <f t="shared" si="12"/>
-        <v>1263.3436892312541</v>
+        <v>1263</v>
       </c>
       <c r="U36">
         <f t="shared" si="12"/>
-        <v>503.4424601586548</v>
+        <v>503</v>
       </c>
       <c r="V36">
         <f t="shared" si="12"/>
-        <v>200.62182037322395</v>
+        <v>200</v>
       </c>
       <c r="W36">
         <f t="shared" si="12"/>
-        <v>79.947795418729754</v>
+        <v>79</v>
       </c>
       <c r="X36">
         <f t="shared" si="10"/>
@@ -5129,47 +5129,47 @@
       </c>
       <c r="M37">
         <f t="shared" si="8"/>
-        <v>14337.716200000001</v>
+        <v>14337</v>
       </c>
       <c r="N37">
         <f t="shared" si="9"/>
-        <v>897.54103412000006</v>
+        <v>897</v>
       </c>
       <c r="O37">
         <f t="shared" si="12"/>
-        <v>56.186068735912009</v>
+        <v>56</v>
       </c>
       <c r="P37">
         <f t="shared" si="12"/>
-        <v>3.5172479028680921</v>
+        <v>3</v>
       </c>
       <c r="Q37">
         <f t="shared" si="12"/>
-        <v>0.22017971871954256</v>
+        <v>0</v>
       </c>
       <c r="R37">
         <f t="shared" si="12"/>
-        <v>1.3783250391843365E-2</v>
+        <v>0</v>
       </c>
       <c r="S37">
         <f t="shared" si="12"/>
-        <v>8.6283147452939472E-4</v>
+        <v>0</v>
       </c>
       <c r="T37">
         <f t="shared" si="12"/>
-        <v>5.4013250305540115E-5</v>
+        <v>0</v>
       </c>
       <c r="U37">
         <f t="shared" si="12"/>
-        <v>3.3812294691268114E-6</v>
+        <v>0</v>
       </c>
       <c r="V37">
         <f t="shared" si="12"/>
-        <v>2.1166496476733841E-7</v>
+        <v>0</v>
       </c>
       <c r="W37">
         <f t="shared" si="12"/>
-        <v>1.3250226794435385E-8</v>
+        <v>0</v>
       </c>
       <c r="X37">
         <f t="shared" si="10"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="Y37" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
@@ -5226,47 +5226,47 @@
       </c>
       <c r="M38">
         <f t="shared" si="8"/>
-        <v>1944367.1146</v>
+        <v>1944367</v>
       </c>
       <c r="N38">
         <f t="shared" si="9"/>
-        <v>1586214.6920906799</v>
+        <v>1586214</v>
       </c>
       <c r="O38">
         <f t="shared" si="12"/>
-        <v>1294033.9458075766</v>
+        <v>1294033</v>
       </c>
       <c r="P38">
         <f t="shared" si="12"/>
-        <v>1055672.892989821</v>
+        <v>1055672</v>
       </c>
       <c r="Q38">
         <f t="shared" si="12"/>
-        <v>861217.94610109599</v>
+        <v>861217</v>
       </c>
       <c r="R38">
         <f t="shared" si="12"/>
-        <v>702581.60042927414</v>
+        <v>702580</v>
       </c>
       <c r="S38">
         <f t="shared" si="12"/>
-        <v>573166.06963020179</v>
+        <v>573164</v>
       </c>
       <c r="T38">
         <f t="shared" si="12"/>
-        <v>467588.87960431859</v>
+        <v>467587</v>
       </c>
       <c r="U38">
         <f t="shared" si="12"/>
-        <v>381459.00798120309</v>
+        <v>381457</v>
       </c>
       <c r="V38">
         <f t="shared" si="12"/>
-        <v>311194.25871106546</v>
+        <v>311192</v>
       </c>
       <c r="W38">
         <f t="shared" si="12"/>
-        <v>253872.27625648718</v>
+        <v>253870</v>
       </c>
       <c r="X38">
         <f t="shared" si="10"/>
@@ -5274,7 +5274,7 @@
       </c>
       <c r="Y38" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -5323,47 +5323,47 @@
       </c>
       <c r="M39">
         <f t="shared" si="8"/>
-        <v>234178.86070000002</v>
+        <v>234178</v>
       </c>
       <c r="N39">
         <f t="shared" si="9"/>
-        <v>62502.33792083001</v>
+        <v>62502</v>
       </c>
       <c r="O39">
         <f t="shared" si="12"/>
-        <v>16681.873991069533</v>
+        <v>16681</v>
       </c>
       <c r="P39">
         <f t="shared" si="12"/>
-        <v>4452.3921682164591</v>
+        <v>4452</v>
       </c>
       <c r="Q39">
         <f t="shared" si="12"/>
-        <v>1188.343469696973</v>
+        <v>1188</v>
       </c>
       <c r="R39">
         <f t="shared" si="12"/>
-        <v>317.16887206212215</v>
+        <v>317</v>
       </c>
       <c r="S39">
         <f t="shared" si="12"/>
-        <v>84.65237195338041</v>
+        <v>84</v>
       </c>
       <c r="T39">
         <f t="shared" si="12"/>
-        <v>22.593718074357234</v>
+        <v>22</v>
       </c>
       <c r="U39">
         <f t="shared" si="12"/>
-        <v>6.030263354045946</v>
+        <v>5</v>
       </c>
       <c r="V39">
         <f t="shared" si="12"/>
-        <v>1.6094772891948632</v>
+        <v>1</v>
       </c>
       <c r="W39">
         <f t="shared" si="12"/>
-        <v>0.42956948848610904</v>
+        <v>0</v>
       </c>
       <c r="X39">
         <f t="shared" si="10"/>
@@ -5371,7 +5371,7 @@
       </c>
       <c r="Y39" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
@@ -5420,47 +5420,47 @@
       </c>
       <c r="M40">
         <f t="shared" si="8"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="N40">
         <f t="shared" si="9"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="O40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="P40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="Q40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="R40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="S40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="T40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="U40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="V40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="W40">
         <f t="shared" si="12"/>
-        <v>33376874.433800001</v>
+        <v>33376874</v>
       </c>
       <c r="X40">
         <f t="shared" si="10"/>
@@ -5517,47 +5517,47 @@
       </c>
       <c r="M41">
         <f t="shared" si="8"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="N41">
         <f t="shared" si="9"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="O41">
-        <f t="shared" ref="O41:W51" si="13">IF(N41&gt;$J41*2, N41, N41*$L41)</f>
-        <v>11676146.7796</v>
+        <f t="shared" ref="O41:W51" si="13">IF(N41&gt;$J41*2, N41, ROUNDDOWN(N41*$L41, 0))</f>
+        <v>11676146</v>
       </c>
       <c r="P41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="Q41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="R41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="S41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="T41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="U41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="V41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="W41">
         <f t="shared" si="13"/>
-        <v>11676146.7796</v>
+        <v>11676146</v>
       </c>
       <c r="X41">
         <f t="shared" si="10"/>
@@ -5614,47 +5614,47 @@
       </c>
       <c r="M42">
         <f t="shared" si="8"/>
-        <v>206.93789999999998</v>
+        <v>206</v>
       </c>
       <c r="N42">
         <f t="shared" si="9"/>
-        <v>1.4278715099999999</v>
+        <v>1</v>
       </c>
       <c r="O42">
         <f t="shared" si="13"/>
-        <v>9.8523134189999993E-3</v>
+        <v>0</v>
       </c>
       <c r="P42">
         <f t="shared" si="13"/>
-        <v>6.7980962591099992E-5</v>
+        <v>0</v>
       </c>
       <c r="Q42">
         <f t="shared" si="13"/>
-        <v>4.6906864187858995E-7</v>
+        <v>0</v>
       </c>
       <c r="R42">
         <f t="shared" si="13"/>
-        <v>3.2365736289622704E-9</v>
+        <v>0</v>
       </c>
       <c r="S42">
         <f t="shared" si="13"/>
-        <v>2.2332358039839664E-11</v>
+        <v>0</v>
       </c>
       <c r="T42">
         <f t="shared" si="13"/>
-        <v>1.5409327047489369E-13</v>
+        <v>0</v>
       </c>
       <c r="U42">
         <f t="shared" si="13"/>
-        <v>1.0632435662767665E-15</v>
+        <v>0</v>
       </c>
       <c r="V42">
         <f t="shared" si="13"/>
-        <v>7.3363806073096888E-18</v>
+        <v>0</v>
       </c>
       <c r="W42">
         <f t="shared" si="13"/>
-        <v>5.0621026190436852E-20</v>
+        <v>0</v>
       </c>
       <c r="X42">
         <f t="shared" si="10"/>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="Y42" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
@@ -5711,47 +5711,47 @@
       </c>
       <c r="M43">
         <f t="shared" si="8"/>
-        <v>116220.91649999999</v>
+        <v>116220</v>
       </c>
       <c r="N43">
         <f t="shared" si="9"/>
-        <v>18583.724548349997</v>
+        <v>18583</v>
       </c>
       <c r="O43">
         <f t="shared" si="13"/>
-        <v>2971.5375552811643</v>
+        <v>2971</v>
       </c>
       <c r="P43">
         <f t="shared" si="13"/>
-        <v>475.14885508945815</v>
+        <v>475</v>
       </c>
       <c r="Q43">
         <f t="shared" si="13"/>
-        <v>75.976301928804347</v>
+        <v>75</v>
       </c>
       <c r="R43">
         <f t="shared" si="13"/>
-        <v>12.148610678415814</v>
+        <v>11</v>
       </c>
       <c r="S43">
         <f t="shared" si="13"/>
-        <v>1.9425628474786885</v>
+        <v>1</v>
       </c>
       <c r="T43">
         <f t="shared" si="13"/>
-        <v>0.31061579931184224</v>
+        <v>0</v>
       </c>
       <c r="U43">
         <f t="shared" si="13"/>
-        <v>4.9667466309963569E-2</v>
+        <v>0</v>
       </c>
       <c r="V43">
         <f t="shared" si="13"/>
-        <v>7.9418278629631734E-3</v>
+        <v>0</v>
       </c>
       <c r="W43">
         <f t="shared" si="13"/>
-        <v>1.2698982752878114E-3</v>
+        <v>0</v>
       </c>
       <c r="X43">
         <f t="shared" si="10"/>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="Y43" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
@@ -5808,47 +5808,47 @@
       </c>
       <c r="M44">
         <f t="shared" si="8"/>
-        <v>1113.5544</v>
+        <v>1113</v>
       </c>
       <c r="N44">
         <f t="shared" si="9"/>
-        <v>16.369249679999999</v>
+        <v>16</v>
       </c>
       <c r="O44">
         <f t="shared" si="13"/>
-        <v>0.24062797029599997</v>
+        <v>0</v>
       </c>
       <c r="P44">
         <f t="shared" si="13"/>
-        <v>3.5372311633511994E-3</v>
+        <v>0</v>
       </c>
       <c r="Q44">
         <f t="shared" si="13"/>
-        <v>5.1997298101262632E-5</v>
+        <v>0</v>
       </c>
       <c r="R44">
         <f t="shared" si="13"/>
-        <v>7.6436028208856064E-7</v>
+        <v>0</v>
       </c>
       <c r="S44">
         <f t="shared" si="13"/>
-        <v>1.1236096146701841E-8</v>
+        <v>0</v>
       </c>
       <c r="T44">
         <f t="shared" si="13"/>
-        <v>1.6517061335651706E-10</v>
+        <v>0</v>
       </c>
       <c r="U44">
         <f t="shared" si="13"/>
-        <v>2.4280080163408007E-12</v>
+        <v>0</v>
       </c>
       <c r="V44">
         <f t="shared" si="13"/>
-        <v>3.5691717840209771E-14</v>
+        <v>0</v>
       </c>
       <c r="W44">
         <f t="shared" si="13"/>
-        <v>5.2466825225108364E-16</v>
+        <v>0</v>
       </c>
       <c r="X44">
         <f t="shared" si="10"/>
@@ -5856,7 +5856,7 @@
       </c>
       <c r="Y44" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
@@ -5905,47 +5905,47 @@
       </c>
       <c r="M45">
         <f t="shared" si="8"/>
-        <v>2448179.5967999999</v>
+        <v>2448179</v>
       </c>
       <c r="N45">
         <f t="shared" si="9"/>
-        <v>2961318.04028928</v>
+        <v>2961317</v>
       </c>
       <c r="O45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="P45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="Q45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="R45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="S45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="T45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="U45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="V45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="W45">
         <f t="shared" si="13"/>
-        <v>3582010.3015339132</v>
+        <v>3582009</v>
       </c>
       <c r="X45">
         <f t="shared" si="10"/>
@@ -6002,47 +6002,47 @@
       </c>
       <c r="M46">
         <f t="shared" si="8"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="N46">
         <f t="shared" si="9"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="O46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="P46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="Q46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="R46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="S46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="T46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="U46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="V46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="W46">
         <f t="shared" si="13"/>
-        <v>4711378.3109999998</v>
+        <v>4711378</v>
       </c>
       <c r="X46">
         <f t="shared" si="10"/>
@@ -6099,47 +6099,47 @@
       </c>
       <c r="M47">
         <f t="shared" si="8"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="N47">
         <f t="shared" si="9"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="O47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="P47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="Q47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="R47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="S47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="T47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="U47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="V47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="W47">
         <f t="shared" si="13"/>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
       <c r="X47">
         <f t="shared" si="10"/>
@@ -6196,47 +6196,47 @@
       </c>
       <c r="M48">
         <f t="shared" si="8"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="N48">
         <f t="shared" si="9"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="O48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="P48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="Q48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="R48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="S48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="T48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="U48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="V48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="W48">
         <f t="shared" si="13"/>
-        <v>11599576.326400001</v>
+        <v>11599576</v>
       </c>
       <c r="X48">
         <f t="shared" si="10"/>
@@ -6293,47 +6293,47 @@
       </c>
       <c r="M49">
         <f t="shared" si="8"/>
-        <v>6026279.3065999998</v>
+        <v>6026279</v>
       </c>
       <c r="N49">
         <f t="shared" si="9"/>
-        <v>6384240.2974120388</v>
+        <v>6384239</v>
       </c>
       <c r="O49">
         <f t="shared" si="13"/>
-        <v>6763464.1710783131</v>
+        <v>6763462</v>
       </c>
       <c r="P49">
         <f t="shared" si="13"/>
-        <v>7165213.9428403638</v>
+        <v>7165211</v>
       </c>
       <c r="Q49">
         <f t="shared" si="13"/>
-        <v>7590827.6510450803</v>
+        <v>7590824</v>
       </c>
       <c r="R49">
         <f t="shared" si="13"/>
-        <v>8041722.813517157</v>
+        <v>8041718</v>
       </c>
       <c r="S49">
         <f t="shared" si="13"/>
-        <v>8519401.1486400757</v>
+        <v>8519396</v>
       </c>
       <c r="T49">
         <f t="shared" si="13"/>
-        <v>9025453.5768692959</v>
+        <v>9025448</v>
       </c>
       <c r="U49">
         <f t="shared" si="13"/>
-        <v>9561565.5193353314</v>
+        <v>9561559</v>
       </c>
       <c r="V49">
         <f t="shared" si="13"/>
-        <v>10129522.511183849</v>
+        <v>10129515</v>
       </c>
       <c r="W49">
         <f t="shared" si="13"/>
-        <v>10731216.148348168</v>
+        <v>10731208</v>
       </c>
       <c r="X49">
         <f t="shared" si="10"/>
@@ -6341,7 +6341,7 @@
       </c>
       <c r="Y49" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
@@ -6390,47 +6390,47 @@
       </c>
       <c r="M50">
         <f t="shared" si="8"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="N50">
         <f t="shared" si="9"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="O50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="P50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="Q50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="R50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="S50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="T50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="U50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="V50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="W50">
         <f t="shared" si="13"/>
-        <v>71920887.238399997</v>
+        <v>71920887</v>
       </c>
       <c r="X50">
         <f t="shared" si="10"/>
@@ -6487,47 +6487,47 @@
       </c>
       <c r="M51">
         <f t="shared" si="8"/>
-        <v>2602010.1455000001</v>
+        <v>2602010</v>
       </c>
       <c r="N51">
         <f t="shared" si="9"/>
-        <v>1854973.03272695</v>
+        <v>1854972</v>
       </c>
       <c r="O51">
         <f t="shared" si="13"/>
-        <v>1322410.2750310425</v>
+        <v>1322409</v>
       </c>
       <c r="P51">
         <f t="shared" si="13"/>
-        <v>942746.28506963013</v>
+        <v>942745</v>
       </c>
       <c r="Q51">
         <f t="shared" si="13"/>
-        <v>672083.82662613934</v>
+        <v>672082</v>
       </c>
       <c r="R51">
         <f t="shared" si="13"/>
-        <v>479128.56000177475</v>
+        <v>479127</v>
       </c>
       <c r="S51">
         <f t="shared" si="13"/>
-        <v>341570.75042526523</v>
+        <v>341569</v>
       </c>
       <c r="T51">
         <f t="shared" si="13"/>
-        <v>243505.78797817157</v>
+        <v>243504</v>
       </c>
       <c r="U51">
         <f t="shared" si="13"/>
-        <v>173595.2762496385</v>
+        <v>173594</v>
       </c>
       <c r="V51">
         <f t="shared" si="13"/>
-        <v>123756.07243836728</v>
+        <v>123755</v>
       </c>
       <c r="W51">
         <f t="shared" si="13"/>
-        <v>88225.704041312027</v>
+        <v>88224</v>
       </c>
       <c r="X51">
         <f t="shared" si="10"/>
@@ -6547,7 +6547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
@@ -6711,7 +6711,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6728,7 +6728,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM(dane!W2:W1000)</f>
-        <v>402395586.84369951</v>
+        <v>402395501</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6737,7 +6737,7 @@
       </c>
       <c r="B3">
         <f>MAX(dane!W2:W1000)</f>
-        <v>105709857.79859999</v>
+        <v>105709857</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6766,7 +6766,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>COUNTIF(dane!Y:Y, TRUE)</f>
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>